<commit_message>
Added MLDM Exercise 02
</commit_message>
<xml_diff>
--- a/2020 Herbstsemester/Stundenplan v0.1.xlsx
+++ b/2020 Herbstsemester/Stundenplan v0.1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FF2753-A010-4B78-9262-4240BCDEF233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEE8864-2471-4E57-B8B4-EBE2F8C2C37F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41130" yWindow="8145" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kursplan" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>KURSPLAN</t>
   </si>
@@ -110,9 +110,6 @@
     <t>EINDEUTIG</t>
   </si>
   <si>
-    <t>Security</t>
-  </si>
-  <si>
     <t>Fribourg</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>Machine Learning</t>
   </si>
   <si>
-    <t>Digitale Nachaltigkeit</t>
-  </si>
-  <si>
     <t>45 MIN</t>
   </si>
   <si>
@@ -144,12 +138,6 @@
   </si>
   <si>
     <t>ASE f2f</t>
-  </si>
-  <si>
-    <t>SEC f2f</t>
-  </si>
-  <si>
-    <t>DN f2f</t>
   </si>
   <si>
     <t>AN online</t>
@@ -1407,7 +1395,7 @@
         <v>0.34375</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I2" s="15"/>
     </row>
@@ -1522,9 +1510,9 @@
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DIENSTAG]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B6&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="7" t="str">
+      <c r="F6" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[MITTWOCH]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B6&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
-        <v>DN f2f</v>
+        <v>0</v>
       </c>
       <c r="G6" s="7" t="str">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DONNERSTAG]])*(ROUNDDOWN($B6,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B6&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
@@ -1556,9 +1544,9 @@
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DIENSTAG]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B7&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="7" t="str">
+      <c r="F7" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[MITTWOCH]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B7&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
-        <v>DN f2f</v>
+        <v>0</v>
       </c>
       <c r="G7" s="7" t="str">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DONNERSTAG]])*(ROUNDDOWN($B7,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B7&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
@@ -1590,9 +1578,9 @@
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DIENSTAG]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B8&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="7" t="str">
+      <c r="F8" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[MITTWOCH]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B8&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
-        <v>DN f2f</v>
+        <v>0</v>
       </c>
       <c r="G8" s="7" t="str">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DONNERSTAG]])*(ROUNDDOWN($B8,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B8&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
@@ -1624,9 +1612,9 @@
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DIENSTAG]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B9&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="7" t="str">
+      <c r="F9" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[MITTWOCH]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B9&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
-        <v>DN f2f</v>
+        <v>0</v>
       </c>
       <c r="G9" s="7" t="str">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DONNERSTAG]])*(ROUNDDOWN($B9,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B9&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
@@ -1726,9 +1714,9 @@
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DIENSTAG]])*(ROUNDDOWN($B12,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B12&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
         <v>DS f2f</v>
       </c>
-      <c r="F12" s="7" t="str">
+      <c r="F12" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[MITTWOCH]])*(ROUNDDOWN($B12,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B12&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
-        <v>SEC f2f</v>
+        <v>0</v>
       </c>
       <c r="G12" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DONNERSTAG]])*(ROUNDDOWN($B12,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B12&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
@@ -1760,9 +1748,9 @@
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DIENSTAG]])*(ROUNDDOWN($B13,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B13&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
         <v>DS f2f</v>
       </c>
-      <c r="F13" s="7" t="str">
+      <c r="F13" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[MITTWOCH]])*(ROUNDDOWN($B13,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B13&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
-        <v>SEC f2f</v>
+        <v>0</v>
       </c>
       <c r="G13" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DONNERSTAG]])*(ROUNDDOWN($B13,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B13&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
@@ -1794,9 +1782,9 @@
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DIENSTAG]])*(ROUNDDOWN($B14,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B14&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
         <v>DS f2f</v>
       </c>
-      <c r="F14" s="7" t="str">
+      <c r="F14" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[MITTWOCH]])*(ROUNDDOWN($B14,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B14&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
-        <v>SEC f2f</v>
+        <v>0</v>
       </c>
       <c r="G14" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DONNERSTAG]])*(ROUNDDOWN($B14,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B14&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
@@ -1828,9 +1816,9 @@
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DIENSTAG]])*(ROUNDDOWN($B15,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B15&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
         <v>DS f2f</v>
       </c>
-      <c r="F15" s="7" t="str">
+      <c r="F15" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[MITTWOCH]])*(ROUNDDOWN($B15,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B15&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
-        <v>SEC f2f</v>
+        <v>0</v>
       </c>
       <c r="G15" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DONNERSTAG]])*(ROUNDDOWN($B15,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B15&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
@@ -1862,9 +1850,9 @@
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DIENSTAG]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B16&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
         <v>DS f2f</v>
       </c>
-      <c r="F16" s="7" t="str">
+      <c r="F16" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[MITTWOCH]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B16&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
-        <v>SEC f2f</v>
+        <v>0</v>
       </c>
       <c r="G16" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DONNERSTAG]])*(ROUNDDOWN($B16,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B16&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
@@ -1896,9 +1884,9 @@
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DIENSTAG]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B17&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
         <v>DS f2f</v>
       </c>
-      <c r="F17" s="7" t="str">
+      <c r="F17" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[MITTWOCH]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B17&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
-        <v>SEC f2f</v>
+        <v>0</v>
       </c>
       <c r="G17" s="7">
         <f>IFERROR(INDEX(Kursliste[],MATCH(SUMPRODUCT((Kursliste[TAG]=Kursplan[[#Headers],[DONNERSTAG]])*(ROUNDDOWN($B17,10)&gt;=ROUNDDOWN(Kursliste[ANFANGSZEIT],10))*($B17&lt;=Kursliste[ENDZEIT]),Kursliste[EINDEUTIG]),Kursliste[EINDEUTIG],0),2),0)</f>
@@ -3339,7 +3327,7 @@
   <dimension ref="B1:H10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3392,16 +3380,16 @@
     </row>
     <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" s="5">
         <v>0.59375</v>
@@ -3416,16 +3404,16 @@
     </row>
     <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="5">
         <v>0.38541666666666669</v>
@@ -3439,48 +3427,24 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="13">
-        <v>0.59375</v>
-      </c>
-      <c r="G5" s="13">
-        <v>0.75</v>
-      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
       <c r="H5" s="2">
         <f>ROW()-ROW(Kursliste[[#Headers],[EINDEUTIG]])</f>
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="13">
-        <v>0.38541666666666669</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0.5</v>
-      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
       <c r="H6" s="2">
         <f>ROW()-ROW(Kursliste[[#Headers],[EINDEUTIG]])</f>
         <v>4</v>
@@ -3488,16 +3452,16 @@
     </row>
     <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="13">
         <v>0.42708333333333331</v>
@@ -3512,16 +3476,16 @@
     </row>
     <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" s="13">
         <v>0.34375</v>

</xml_diff>